<commit_message>
relatório prestação de contas 2023
</commit_message>
<xml_diff>
--- a/Gestão do Projeto/PlanodeTrabalho/Anexo 1. Matriz da Gestão de Risco.xlsx
+++ b/Gestão do Projeto/PlanodeTrabalho/Anexo 1. Matriz da Gestão de Risco.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/1.RepositorioSemantico/Terminologias/OBM/Horus_CMED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documentos\ips-brasil-documentos\Gestão do Projeto\PlanodeTrabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C28263DF-D40F-6D48-881D-0B35882D2890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="756" windowWidth="30240" windowHeight="17904"/>
   </bookViews>
   <sheets>
     <sheet name="Diagnóstico Risco" sheetId="4" r:id="rId1"/>
@@ -21,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fórmula para Risco'!$A$1:$C$26</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
   </numFmts>
@@ -1308,7 +1308,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -1724,25 +1724,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBED67F-F37A-401D-B1E6-2DA04306A030}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="K13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="30.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="30.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="30.5" style="1"/>
-    <col min="6" max="8" width="30.5" style="40"/>
-    <col min="9" max="16384" width="30.5" style="1"/>
+    <col min="1" max="5" width="30.44140625" style="1"/>
+    <col min="6" max="8" width="30.44140625" style="40"/>
+    <col min="9" max="16384" width="30.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="94" t="s">
         <v>1</v>
       </c>
@@ -1769,12 +1769,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N4" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="32" t="s">
         <v>4</v>
@@ -1816,7 +1816,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="56" t="s">
         <v>17</v>
@@ -1859,7 +1859,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="91" t="s">
         <v>29</v>
@@ -1902,7 +1902,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="92"/>
       <c r="C8" s="55" t="s">
@@ -1943,7 +1943,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="92"/>
       <c r="C9" s="55" t="s">
@@ -1983,7 +1983,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="93"/>
       <c r="C10" s="77" t="s">
@@ -2023,7 +2023,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="91" t="s">
         <v>93</v>
@@ -2066,7 +2066,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="92"/>
       <c r="C12" s="70" t="s">
@@ -2107,7 +2107,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="92"/>
       <c r="C13" s="70" t="s">
@@ -2148,7 +2148,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="92"/>
       <c r="C14" s="81" t="s">
@@ -2189,7 +2189,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="92"/>
       <c r="C15" s="80" t="s">
@@ -2230,7 +2230,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="78" t="s">
         <v>103</v>
@@ -2273,7 +2273,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="82"/>
       <c r="C17" s="58"/>
@@ -2289,7 +2289,7 @@
       <c r="M17" s="84"/>
       <c r="N17" s="86"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="82"/>
       <c r="C18" s="58"/>
@@ -2305,7 +2305,7 @@
       <c r="M18" s="84"/>
       <c r="N18" s="86"/>
     </row>
-    <row r="19" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="58" t="s">
         <v>37</v>
       </c>
@@ -2325,7 +2325,7 @@
       <c r="M19" s="5"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="33"/>
       <c r="C20" s="59" t="s">
@@ -2343,7 +2343,7 @@
       <c r="M20" s="61"/>
       <c r="N20" s="5"/>
     </row>
-    <row r="21" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="33"/>
       <c r="C21" s="57"/>
@@ -2359,7 +2359,7 @@
       <c r="M21" s="63"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="57" t="s">
         <v>40</v>
       </c>
@@ -2379,7 +2379,7 @@
       <c r="M22" s="57"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="34"/>
       <c r="C23" s="66" t="s">
@@ -2399,7 +2399,7 @@
       </c>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="47"/>
       <c r="C24" s="66" t="s">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="47"/>
       <c r="C25" s="66" t="s">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="47"/>
       <c r="C26" s="66" t="s">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="47"/>
       <c r="C27" s="67" t="s">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="48"/>
       <c r="C28" s="69"/>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="69"/>
       <c r="C29" s="57"/>
@@ -2513,7 +2513,7 @@
       <c r="M29" s="69"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="57" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +2533,7 @@
       <c r="M30" s="57"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="34"/>
       <c r="C31" s="66" t="s">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="9"/>
       <c r="C32" s="66" t="s">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="9"/>
       <c r="C33" s="66" t="s">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="N33" s="5"/>
     </row>
-    <row r="34" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="9"/>
       <c r="C34" s="66" t="s">
@@ -2613,7 +2613,7 @@
       </c>
       <c r="N34" s="5"/>
     </row>
-    <row r="35" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="9"/>
       <c r="C35" s="67" t="s">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="N35" s="5"/>
     </row>
-    <row r="36" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="35"/>
       <c r="C36" s="69"/>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="N36" s="5"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="69"/>
       <c r="C37" s="5"/>
@@ -2667,7 +2667,7 @@
       <c r="M37" s="69"/>
       <c r="N37" s="5"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="45"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2683,7 +2683,7 @@
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="45"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2699,7 +2699,7 @@
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="45"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2715,7 +2715,7 @@
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="45"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2731,7 +2731,7 @@
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="5"/>
       <c r="C42" s="95" t="s">
@@ -2749,7 +2749,7 @@
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="36"/>
       <c r="C43" s="100" t="s">
@@ -2767,7 +2767,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="16"/>
       <c r="C44" s="100" t="s">
@@ -2785,7 +2785,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="5"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="12"/>
       <c r="C45" s="100" t="s">
@@ -2803,7 +2803,7 @@
       <c r="M45" s="2"/>
       <c r="N45" s="5"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="17"/>
       <c r="C46" s="102" t="s">
@@ -2821,7 +2821,7 @@
       <c r="M46" s="2"/>
       <c r="N46" s="5"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="37"/>
       <c r="C47" s="46"/>
@@ -2837,7 +2837,7 @@
       <c r="M47" s="2"/>
       <c r="N47" s="5"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="46"/>
       <c r="C48" s="57"/>
@@ -2853,7 +2853,7 @@
       <c r="M48" s="2"/>
       <c r="N48" s="5"/>
     </row>
-    <row r="49" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="57" t="s">
         <v>60</v>
       </c>
@@ -2871,7 +2871,7 @@
       <c r="M49" s="57"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="98" t="s">
         <v>61</v>
       </c>
@@ -2895,7 +2895,7 @@
       <c r="M50" s="2"/>
       <c r="N50" s="5"/>
     </row>
-    <row r="51" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="99"/>
       <c r="B51" s="9"/>
       <c r="C51" s="16" t="s">
@@ -2921,7 +2921,7 @@
       <c r="M51" s="2"/>
       <c r="N51" s="5"/>
     </row>
-    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="99"/>
       <c r="B52" s="9"/>
       <c r="C52" s="16" t="s">
@@ -2947,7 +2947,7 @@
       <c r="M52" s="2"/>
       <c r="N52" s="5"/>
     </row>
-    <row r="53" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="99"/>
       <c r="B53" s="9"/>
       <c r="C53" s="16" t="s">
@@ -2973,7 +2973,7 @@
       <c r="M53" s="2"/>
       <c r="N53" s="5"/>
     </row>
-    <row r="54" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="99"/>
       <c r="B54" s="9"/>
       <c r="C54" s="16" t="s">
@@ -2999,7 +2999,7 @@
       <c r="M54" s="2"/>
       <c r="N54" s="5"/>
     </row>
-    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="99"/>
       <c r="B55" s="9"/>
       <c r="C55" s="20" t="s">
@@ -3025,7 +3025,7 @@
       <c r="M55" s="2"/>
       <c r="N55" s="5"/>
     </row>
-    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="99"/>
       <c r="B56" s="38"/>
       <c r="C56" s="72" t="s">
@@ -3047,7 +3047,7 @@
       <c r="M56" s="2"/>
       <c r="N56" s="5"/>
     </row>
-    <row r="57" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="22"/>
       <c r="B57" s="2"/>
       <c r="C57" s="69"/>
@@ -3063,7 +3063,7 @@
       <c r="M57" s="2"/>
       <c r="N57" s="5"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="69"/>
       <c r="C58" s="73"/>
@@ -3079,7 +3079,7 @@
       <c r="M58" s="2"/>
       <c r="N58" s="5"/>
     </row>
-    <row r="59" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="73" t="s">
         <v>70</v>
       </c>
@@ -3099,7 +3099,7 @@
       <c r="M59" s="5"/>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="39"/>
       <c r="C60" s="66" t="s">
@@ -3117,7 +3117,7 @@
       <c r="M60" s="75"/>
       <c r="N60" s="5"/>
     </row>
-    <row r="61" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="66" t="s">
@@ -3135,7 +3135,7 @@
       <c r="M61" s="71"/>
       <c r="N61" s="5"/>
     </row>
-    <row r="62" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="9"/>
       <c r="C62" s="66" t="s">
@@ -3153,7 +3153,7 @@
       <c r="M62" s="71"/>
       <c r="N62" s="5"/>
     </row>
-    <row r="63" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="9"/>
       <c r="C63" s="67" t="s">
@@ -3171,7 +3171,7 @@
       <c r="M63" s="71"/>
       <c r="N63" s="5"/>
     </row>
-    <row r="64" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="35"/>
       <c r="C64" s="45"/>
@@ -3187,7 +3187,7 @@
       <c r="M64" s="76"/>
       <c r="N64" s="5"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="45"/>
       <c r="C65" s="2"/>
@@ -3203,7 +3203,7 @@
       <c r="M65" s="45"/>
       <c r="N65" s="5"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="H66" s="9"/>
@@ -3241,7 +3241,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C15" r:id="rId1" display="mailto:gabriel.gaoliveira@hsl.org.br" xr:uid="{6F59F6B6-71F9-2E48-8E2D-579EC9C4B88F}"/>
+    <hyperlink ref="C15" r:id="rId1" display="mailto:gabriel.gaoliveira@hsl.org.br"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3250,25 +3250,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>75</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>25</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>67</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
         <v>79</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>67</v>
       </c>
@@ -3327,7 +3327,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>79</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>80</v>
       </c>
@@ -3354,7 +3354,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>80</v>
       </c>
@@ -3367,7 +3367,7 @@
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>80</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="F9"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>35</v>
       </c>
@@ -3393,7 +3393,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
         <v>80</v>
       </c>
@@ -3406,7 +3406,7 @@
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>35</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>25</v>
       </c>
@@ -3432,7 +3432,7 @@
       <c r="F13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>67</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="F14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>67</v>
       </c>
@@ -3458,7 +3458,7 @@
       <c r="F15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>79</v>
       </c>
@@ -3471,7 +3471,7 @@
       <c r="F16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>80</v>
       </c>
@@ -3484,7 +3484,7 @@
       <c r="F17"/>
       <c r="G17"/>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>35</v>
       </c>
@@ -3497,7 +3497,7 @@
       <c r="F18"/>
       <c r="G18"/>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>35</v>
       </c>
@@ -3510,7 +3510,7 @@
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>25</v>
       </c>
@@ -3523,7 +3523,7 @@
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
         <v>35</v>
       </c>
@@ -3536,7 +3536,7 @@
       <c r="F21"/>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>25</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>25</v>
       </c>
@@ -3562,7 +3562,7 @@
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
         <v>67</v>
       </c>
@@ -3575,7 +3575,7 @@
       <c r="F24"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>79</v>
       </c>
@@ -3588,7 +3588,7 @@
       <c r="F25"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
         <v>79</v>
       </c>
@@ -3601,138 +3601,138 @@
       <c r="F26"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F27"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F28"/>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F29"/>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F30"/>
       <c r="G30"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F31"/>
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F32"/>
       <c r="G32"/>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F39"/>
       <c r="G39"/>
     </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F41" s="15"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F42" s="15"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F43" s="17"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F44" s="12"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F45" s="12"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F46" s="20"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F47"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F48"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F49"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F50"/>
       <c r="G50"/>
     </row>
-    <row r="51" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F51"/>
       <c r="G51"/>
     </row>
-    <row r="52" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F52"/>
       <c r="G52"/>
     </row>
-    <row r="53" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F53"/>
       <c r="G53"/>
     </row>
-    <row r="54" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F54"/>
       <c r="G54"/>
     </row>
-    <row r="55" spans="6:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F55"/>
       <c r="G55"/>
     </row>
-    <row r="56" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D56">
+  <sortState ref="A2:D56">
     <sortCondition ref="C2:C56"/>
   </sortState>
   <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:G6" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F6:G6">
       <formula1>"1,2,5,8,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F7" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F7">
       <formula1>"Muito baixa,Baixa,Média,Alta,Muito alta"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G7" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G7">
       <formula1>"Muito baixo,Baixo,Médio,Alto,Muito alto"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3742,19 +3742,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="105" t="s">
         <v>60</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="K1" s="105"/>
       <c r="L1" s="105"/>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="98" t="s">
         <v>61</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="99"/>
       <c r="B3" s="25">
         <v>10</v>
@@ -3820,7 +3820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="99"/>
       <c r="B4" s="25">
         <v>2</v>
@@ -3851,7 +3851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="99"/>
       <c r="B5" s="25">
         <v>5</v>
@@ -3882,7 +3882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="99"/>
       <c r="B6" s="25">
         <v>8</v>
@@ -3913,7 +3913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="99"/>
       <c r="B7" s="25">
         <v>2</v>
@@ -3941,7 +3941,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="99"/>
       <c r="B8" s="25">
         <v>1</v>
@@ -3977,6 +3977,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="343baba5-3cff-45e4-9347-222e64391087">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ac44d7d8-a149-432c-a72c-2d3b3d2b8d35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DB625EBEAB62DA438180CD0344175DCD" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c616db548dd7053096bc9d3c1fea1cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="343baba5-3cff-45e4-9347-222e64391087" xmlns:ns3="ac44d7d8-a149-432c-a72c-2d3b3d2b8d35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="671e8f80c16e47d7001ce2019891b8ed" ns2:_="" ns3:_="">
     <xsd:import namespace="343baba5-3cff-45e4-9347-222e64391087"/>
@@ -4193,27 +4213,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D2B186D-6FC4-4F7A-9C2F-ACFB37C799E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ac44d7d8-a149-432c-a72c-2d3b3d2b8d35"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="343baba5-3cff-45e4-9347-222e64391087"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="343baba5-3cff-45e4-9347-222e64391087">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ac44d7d8-a149-432c-a72c-2d3b3d2b8d35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75F28FB3-CFB3-473B-8A6C-7289F0985AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4975586A-DC85-4C9D-8F11-1B3AF25CC416}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4230,29 +4255,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75F28FB3-CFB3-473B-8A6C-7289F0985AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D2B186D-6FC4-4F7A-9C2F-ACFB37C799E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ac44d7d8-a149-432c-a72c-2d3b3d2b8d35"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="343baba5-3cff-45e4-9347-222e64391087"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>